<commit_message>
fix: adjust short option PnL logic and patch IV bug
</commit_message>
<xml_diff>
--- a/Black–Scholes cacultor.xlsx
+++ b/Black–Scholes cacultor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sofjk\Desktop\Hedge\option_hedge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8329E9-188F-43B9-AABD-EC15F61AED95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C76E35-3154-4850-9CBA-4E917E35020F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11568" yWindow="1548" windowWidth="7500" windowHeight="9960" xr2:uid="{4D6E4BC2-ACBD-4A5A-8BED-4FEB766A38C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4D6E4BC2-ACBD-4A5A-8BED-4FEB766A38C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5E3A07-91F0-4D9C-93C2-5C37F6A770A0}">
   <dimension ref="B3:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="G10">
-        <v>135</v>
+        <v>135.4</v>
       </c>
       <c r="J10" t="s">
         <v>21</v>
@@ -970,7 +970,7 @@
         <v>5</v>
       </c>
       <c r="G11">
-        <v>113</v>
+        <v>140</v>
       </c>
       <c r="J11" t="s">
         <v>20</v>
@@ -984,8 +984,8 @@
         <v>6</v>
       </c>
       <c r="G12" s="5">
-        <f>15/365</f>
-        <v>4.1095890410958902E-2</v>
+        <f>4/365</f>
+        <v>1.0958904109589041E-2</v>
       </c>
       <c r="K12" s="10"/>
     </row>
@@ -1005,7 +1005,7 @@
         <v>8</v>
       </c>
       <c r="G14" s="8">
-        <v>0.63</v>
+        <v>0.4622</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.3">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="G17">
         <f>(LN(G10/G11)+(G15-G13+0.5*G14^2)*G12)/(G14*SQRT(G12))</f>
-        <v>1.4711873245932876</v>
+        <v>-0.65609467342384475</v>
       </c>
       <c r="I17" t="str">
         <f ca="1">_xlfn.FORMULATEXT(G17)</f>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="G18">
         <f>G17-G14*SQRT(G12)</f>
-        <v>1.3434729600757849</v>
+        <v>-0.70447998082808416</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ref="I18:I22" ca="1" si="0">_xlfn.FORMULATEXT(G18)</f>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="G19">
         <f>_xlfn.NORM.S.DIST(G17,TRUE)</f>
-        <v>0.92937976793246768</v>
+        <v>0.255881605722453</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="G20">
         <f>_xlfn.NORM.S.DIST(G18,TRUE)</f>
-        <v>0.91044056202149437</v>
+        <v>0.24056695641804965</v>
       </c>
       <c r="I20" t="str">
         <f ca="1">_xlfn.FORMULATEXT(G20)</f>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="G21">
         <f>_xlfn.NORM.S.DIST(-G17,TRUE)</f>
-        <v>7.062023206753236E-2</v>
+        <v>0.744118394277547</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="G22">
         <f>_xlfn.NORM.S.DIST(-G18,TRUE)</f>
-        <v>8.9559437978505602E-2</v>
+        <v>0.7594330435819503</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="G23">
         <f>_xlfn.NORM.S.DIST(G17,FALSE)</f>
-        <v>0.13518181819448502</v>
+        <v>0.32168944882638989</v>
       </c>
     </row>
     <row r="24" spans="3:19" x14ac:dyDescent="0.3">
@@ -1134,14 +1134,14 @@
       </c>
       <c r="G27" s="4">
         <f>G10*EXP(-G13*G12)*G19-G11*EXP(-G15*G12)*G20</f>
-        <v>22.77656648204281</v>
+        <v>0.98360042790101687</v>
       </c>
       <c r="H27" t="s">
         <v>24</v>
       </c>
       <c r="I27" s="4">
         <f>EXP(-G13*G12)*G19</f>
-        <v>0.92937976793246768</v>
+        <v>0.255881605722453</v>
       </c>
       <c r="K27" t="s">
         <v>22</v>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="N27" s="4">
         <f>EXP(-G13*G12)*G23/(G10*G14*SQRT(G12))</f>
-        <v>7.8405182159709107E-3</v>
+        <v>4.9102617965149316E-2</v>
       </c>
     </row>
     <row r="28" spans="3:19" x14ac:dyDescent="0.3">
@@ -1160,18 +1160,18 @@
       </c>
       <c r="G28" s="4">
         <f>G11*EXP(-G15*G12)*G22-G10*EXP(-G13*G12)*G21</f>
-        <v>0.56778698833648988</v>
+        <v>5.5145763530443759</v>
       </c>
       <c r="H28" t="s">
         <v>25</v>
       </c>
       <c r="I28" s="4">
         <f>-G21*EXP(-G13*G12)</f>
-        <v>-7.062023206753236E-2</v>
+        <v>-0.744118394277547</v>
       </c>
       <c r="J28" s="4">
         <f>I27-1</f>
-        <v>-7.0620232067532318E-2</v>
+        <v>-0.744118394277547</v>
       </c>
       <c r="K28" t="s">
         <v>23</v>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="N28" s="4">
         <f>G24*G23*G10*G14*SQRT(G12)</f>
-        <v>2.3307291006789499</v>
+        <v>2.107506804620368</v>
       </c>
     </row>
     <row r="30" spans="3:19" x14ac:dyDescent="0.3">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="G30" s="4">
         <f>G27-G28</f>
-        <v>22.20877949370632</v>
+        <v>-4.530975925143359</v>
       </c>
     </row>
     <row r="31" spans="3:19" x14ac:dyDescent="0.3">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="G31" s="4">
         <f>G10-G11*EXP(-G15*G12)</f>
-        <v>22.208779493706317</v>
+        <v>-4.5309759251433661</v>
       </c>
       <c r="I31" s="4">
         <v>2.4464803229450141</v>
@@ -1215,7 +1215,7 @@
     <row r="32" spans="3:19" x14ac:dyDescent="0.3">
       <c r="G32">
         <f>G11*EXP(-G15*G12)</f>
-        <v>112.79122050629368</v>
+        <v>139.93097592514337</v>
       </c>
       <c r="I32" s="4"/>
     </row>

</xml_diff>